<commit_message>
[Edited]: Update Excel Reward
</commit_message>
<xml_diff>
--- a/data/reward.xlsx
+++ b/data/reward.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/BAAC_DATA/@Working_Y63/Training/CodeCampUpSkillBatch1/Project/Group/final-americano-api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA7EFC0-0C8C-AB40-B0EE-E64D7DDA8792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1CAE97-656F-5244-9549-48F96088170D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RewardData" sheetId="3" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="42">
   <si>
     <t>1</t>
   </si>
@@ -138,6 +138,9 @@
     <t>5000</t>
   </si>
   <si>
+    <t>2020-07-16</t>
+  </si>
+  <si>
     <t>0234812</t>
   </si>
   <si>
@@ -176,12 +179,15 @@
   <si>
     <t>0515103</t>
   </si>
+  <si>
+    <t>2020-08-16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +216,13 @@
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -269,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -291,9 +304,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="C262" sqref="C262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -665,8 +675,8 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>44059</v>
+      <c r="A2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -682,8 +692,8 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
-        <v>44059</v>
+      <c r="A3" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -696,8 +706,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
-        <v>44059</v>
+      <c r="A4" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -710,8 +720,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>44059</v>
+      <c r="A5" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -724,8 +734,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>44059</v>
+      <c r="A6" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
@@ -743,8 +753,8 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>44059</v>
+      <c r="A7" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
@@ -764,8 +774,8 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>44059</v>
+      <c r="A8" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -783,8 +793,8 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>44059</v>
+      <c r="A9" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>3</v>
@@ -802,8 +812,8 @@
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>44059</v>
+      <c r="A10" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -821,8 +831,8 @@
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>44059</v>
+      <c r="A11" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -835,8 +845,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>44059</v>
+      <c r="A12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -849,8 +859,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>44059</v>
+      <c r="A13" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -863,8 +873,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>44059</v>
+      <c r="A14" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B14" s="3">
         <v>3</v>
@@ -877,8 +887,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
-        <v>44059</v>
+      <c r="A15" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -891,8 +901,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>44059</v>
+      <c r="A16" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
@@ -905,8 +915,8 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
-        <v>44059</v>
+      <c r="A17" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -919,8 +929,8 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
-        <v>44059</v>
+      <c r="A18" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>7</v>
@@ -933,8 +943,8 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
-        <v>44059</v>
+      <c r="A19" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
@@ -947,8 +957,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
-        <v>44059</v>
+      <c r="A20" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>7</v>
@@ -961,8 +971,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
-        <v>44059</v>
+      <c r="A21" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>7</v>
@@ -975,8 +985,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="8">
-        <v>44059</v>
+      <c r="A22" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
@@ -989,8 +999,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="8">
-        <v>44059</v>
+      <c r="A23" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -1003,8 +1013,8 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="8">
-        <v>44059</v>
+      <c r="A24" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>7</v>
@@ -1017,8 +1027,8 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="8">
-        <v>44059</v>
+      <c r="A25" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>7</v>
@@ -1031,8 +1041,8 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
-        <v>44059</v>
+      <c r="A26" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>7</v>
@@ -1045,8 +1055,8 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="8">
-        <v>44059</v>
+      <c r="A27" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>7</v>
@@ -1059,8 +1069,8 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="8">
-        <v>44059</v>
+      <c r="A28" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>7</v>
@@ -1073,8 +1083,8 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="8">
-        <v>44059</v>
+      <c r="A29" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>7</v>
@@ -1087,8 +1097,8 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
-        <v>44059</v>
+      <c r="A30" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>7</v>
@@ -1101,8 +1111,8 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
-        <v>44059</v>
+      <c r="A31" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>7</v>
@@ -1120,8 +1130,8 @@
       <c r="M31" s="7"/>
     </row>
     <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>44059</v>
+      <c r="A32" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>7</v>
@@ -1139,8 +1149,8 @@
       <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
-        <v>44059</v>
+      <c r="A33" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>7</v>
@@ -1158,8 +1168,8 @@
       <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>44059</v>
+      <c r="A34" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>7</v>
@@ -1177,8 +1187,8 @@
       <c r="M34" s="7"/>
     </row>
     <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
-        <v>44059</v>
+      <c r="A35" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>7</v>
@@ -1196,8 +1206,8 @@
       <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
-        <v>44059</v>
+      <c r="A36" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>13</v>
@@ -1215,8 +1225,8 @@
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
-        <v>44059</v>
+      <c r="A37" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>13</v>
@@ -1234,8 +1244,8 @@
       <c r="M37" s="7"/>
     </row>
     <row r="38" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
-        <v>44059</v>
+      <c r="A38" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>13</v>
@@ -1253,8 +1263,8 @@
       <c r="M38" s="7"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
-        <v>44059</v>
+      <c r="A39" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>13</v>
@@ -1272,8 +1282,8 @@
       <c r="M39" s="7"/>
     </row>
     <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
-        <v>44059</v>
+      <c r="A40" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>13</v>
@@ -1291,8 +1301,8 @@
       <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
-        <v>44059</v>
+      <c r="A41" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>13</v>
@@ -1310,8 +1320,8 @@
       <c r="M41" s="7"/>
     </row>
     <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
-        <v>44059</v>
+      <c r="A42" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>13</v>
@@ -1329,8 +1339,8 @@
       <c r="M42" s="7"/>
     </row>
     <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
-        <v>44059</v>
+      <c r="A43" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>13</v>
@@ -1348,8 +1358,8 @@
       <c r="M43" s="7"/>
     </row>
     <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
-        <v>44059</v>
+      <c r="A44" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>13</v>
@@ -1367,8 +1377,8 @@
       <c r="M44" s="7"/>
     </row>
     <row r="45" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
-        <v>44059</v>
+      <c r="A45" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>13</v>
@@ -1386,8 +1396,8 @@
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
-        <v>44059</v>
+      <c r="A46" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>13</v>
@@ -1405,8 +1415,8 @@
       <c r="M46" s="7"/>
     </row>
     <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
-        <v>44059</v>
+      <c r="A47" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>13</v>
@@ -1424,8 +1434,8 @@
       <c r="M47" s="7"/>
     </row>
     <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
-        <v>44059</v>
+      <c r="A48" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>13</v>
@@ -1443,8 +1453,8 @@
       <c r="M48" s="7"/>
     </row>
     <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
-        <v>44059</v>
+      <c r="A49" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>13</v>
@@ -1462,8 +1472,8 @@
       <c r="M49" s="7"/>
     </row>
     <row r="50" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
-        <v>44059</v>
+      <c r="A50" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>13</v>
@@ -1481,8 +1491,8 @@
       <c r="M50" s="7"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="8">
-        <v>44059</v>
+      <c r="A51" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>13</v>
@@ -1495,8 +1505,8 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="8">
-        <v>44059</v>
+      <c r="A52" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>13</v>
@@ -1509,8 +1519,8 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="8">
-        <v>44059</v>
+      <c r="A53" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>13</v>
@@ -1523,8 +1533,8 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="8">
-        <v>44059</v>
+      <c r="A54" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>13</v>
@@ -1537,8 +1547,8 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="8">
-        <v>44059</v>
+      <c r="A55" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>13</v>
@@ -1551,8 +1561,8 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="8">
-        <v>44059</v>
+      <c r="A56" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>13</v>
@@ -1565,8 +1575,8 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="8">
-        <v>44059</v>
+      <c r="A57" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>13</v>
@@ -1579,8 +1589,8 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A58" s="8">
-        <v>44059</v>
+      <c r="A58" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>13</v>
@@ -1593,8 +1603,8 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="8">
-        <v>44059</v>
+      <c r="A59" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>13</v>
@@ -1607,8 +1617,8 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" s="8">
-        <v>44059</v>
+      <c r="A60" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>13</v>
@@ -1621,8 +1631,8 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A61" s="8">
-        <v>44059</v>
+      <c r="A61" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>13</v>
@@ -1635,8 +1645,8 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" s="8">
-        <v>44059</v>
+      <c r="A62" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>13</v>
@@ -1649,8 +1659,8 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="8">
-        <v>44059</v>
+      <c r="A63" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>13</v>
@@ -1663,8 +1673,8 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" s="8">
-        <v>44059</v>
+      <c r="A64" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>13</v>
@@ -1677,8 +1687,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="8">
-        <v>44059</v>
+      <c r="A65" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>13</v>
@@ -1691,8 +1701,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="8">
-        <v>44059</v>
+      <c r="A66" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>13</v>
@@ -1705,8 +1715,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="8">
-        <v>44059</v>
+      <c r="A67" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>13</v>
@@ -1719,8 +1729,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="8">
-        <v>44059</v>
+      <c r="A68" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>13</v>
@@ -1733,8 +1743,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="8">
-        <v>44059</v>
+      <c r="A69" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>13</v>
@@ -1747,8 +1757,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="8">
-        <v>44059</v>
+      <c r="A70" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>13</v>
@@ -1761,8 +1771,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="8">
-        <v>44059</v>
+      <c r="A71" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>13</v>
@@ -1775,8 +1785,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="8">
-        <v>44059</v>
+      <c r="A72" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>13</v>
@@ -1789,8 +1799,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="8">
-        <v>44059</v>
+      <c r="A73" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>13</v>
@@ -1803,8 +1813,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="8">
-        <v>44059</v>
+      <c r="A74" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>13</v>
@@ -1817,8 +1827,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="8">
-        <v>44059</v>
+      <c r="A75" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>13</v>
@@ -1831,8 +1841,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="8">
-        <v>44059</v>
+      <c r="A76" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>13</v>
@@ -1845,8 +1855,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="8">
-        <v>44059</v>
+      <c r="A77" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>13</v>
@@ -1859,8 +1869,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="8">
-        <v>44059</v>
+      <c r="A78" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>13</v>
@@ -1873,8 +1883,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="8">
-        <v>44059</v>
+      <c r="A79" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>13</v>
@@ -1887,8 +1897,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="8">
-        <v>44059</v>
+      <c r="A80" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>13</v>
@@ -1901,8 +1911,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="8">
-        <v>44059</v>
+      <c r="A81" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>13</v>
@@ -1915,8 +1925,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="8">
-        <v>44059</v>
+      <c r="A82" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>13</v>
@@ -1929,8 +1939,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="8">
-        <v>44059</v>
+      <c r="A83" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>13</v>
@@ -1943,8 +1953,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="8">
-        <v>44059</v>
+      <c r="A84" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>13</v>
@@ -1957,8 +1967,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="8">
-        <v>44059</v>
+      <c r="A85" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>13</v>
@@ -1971,8 +1981,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="8">
-        <v>44059</v>
+      <c r="A86" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>13</v>
@@ -1985,8 +1995,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="8">
-        <v>44059</v>
+      <c r="A87" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>13</v>
@@ -1999,8 +2009,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="8">
-        <v>44059</v>
+      <c r="A88" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>13</v>
@@ -2013,8 +2023,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="8">
-        <v>44059</v>
+      <c r="A89" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>13</v>
@@ -2027,8 +2037,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="8">
-        <v>44059</v>
+      <c r="A90" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>13</v>
@@ -2041,8 +2051,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="8">
-        <v>44059</v>
+      <c r="A91" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>13</v>
@@ -2055,8 +2065,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="8">
-        <v>44059</v>
+      <c r="A92" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>13</v>
@@ -2069,8 +2079,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="8">
-        <v>44059</v>
+      <c r="A93" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>13</v>
@@ -2083,8 +2093,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="8">
-        <v>44059</v>
+      <c r="A94" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>13</v>
@@ -2097,8 +2107,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="8">
-        <v>44059</v>
+      <c r="A95" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>13</v>
@@ -2111,8 +2121,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A96" s="8">
-        <v>44059</v>
+      <c r="A96" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>13</v>
@@ -2125,8 +2135,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="8">
-        <v>44059</v>
+      <c r="A97" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>13</v>
@@ -2139,8 +2149,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="8">
-        <v>44059</v>
+      <c r="A98" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>13</v>
@@ -2153,8 +2163,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="8">
-        <v>44059</v>
+      <c r="A99" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>13</v>
@@ -2167,8 +2177,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="8">
-        <v>44059</v>
+      <c r="A100" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>13</v>
@@ -2181,8 +2191,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="8">
-        <v>44059</v>
+      <c r="A101" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>13</v>
@@ -2195,8 +2205,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="8">
-        <v>44059</v>
+      <c r="A102" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>13</v>
@@ -2209,8 +2219,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="8">
-        <v>44059</v>
+      <c r="A103" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>13</v>
@@ -2223,8 +2233,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="8">
-        <v>44059</v>
+      <c r="A104" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>13</v>
@@ -2237,8 +2247,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="8">
-        <v>44059</v>
+      <c r="A105" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>13</v>
@@ -2251,8 +2261,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="8">
-        <v>44059</v>
+      <c r="A106" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>13</v>
@@ -2265,8 +2275,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="8">
-        <v>44059</v>
+      <c r="A107" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>13</v>
@@ -2279,8 +2289,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="8">
-        <v>44059</v>
+      <c r="A108" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>13</v>
@@ -2293,8 +2303,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="8">
-        <v>44059</v>
+      <c r="A109" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>13</v>
@@ -2307,8 +2317,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="8">
-        <v>44059</v>
+      <c r="A110" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>13</v>
@@ -2321,8 +2331,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="8">
-        <v>44059</v>
+      <c r="A111" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>13</v>
@@ -2335,8 +2345,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="8">
-        <v>44059</v>
+      <c r="A112" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>13</v>
@@ -2349,8 +2359,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="8">
-        <v>44059</v>
+      <c r="A113" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>13</v>
@@ -2363,8 +2373,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="8">
-        <v>44059</v>
+      <c r="A114" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>13</v>
@@ -2377,8 +2387,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="8">
-        <v>44059</v>
+      <c r="A115" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>13</v>
@@ -2391,8 +2401,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A116" s="8">
-        <v>44059</v>
+      <c r="A116" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>13</v>
@@ -2405,8 +2415,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="8">
-        <v>44059</v>
+      <c r="A117" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>13</v>
@@ -2419,8 +2429,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="8">
-        <v>44059</v>
+      <c r="A118" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>13</v>
@@ -2433,8 +2443,8 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" s="8">
-        <v>44059</v>
+      <c r="A119" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>13</v>
@@ -2447,8 +2457,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="8">
-        <v>44059</v>
+      <c r="A120" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>13</v>
@@ -2461,8 +2471,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="8">
-        <v>44059</v>
+      <c r="A121" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>13</v>
@@ -2475,8 +2485,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="8">
-        <v>44059</v>
+      <c r="A122" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>13</v>
@@ -2489,8 +2499,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="8">
-        <v>44059</v>
+      <c r="A123" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>13</v>
@@ -2503,8 +2513,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="8">
-        <v>44059</v>
+      <c r="A124" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>13</v>
@@ -2517,8 +2527,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="8">
-        <v>44059</v>
+      <c r="A125" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>13</v>
@@ -2531,8 +2541,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="8">
-        <v>44059</v>
+      <c r="A126" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>13</v>
@@ -2545,8 +2555,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="8">
-        <v>44059</v>
+      <c r="A127" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>13</v>
@@ -2559,8 +2569,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="8">
-        <v>44059</v>
+      <c r="A128" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>13</v>
@@ -2573,8 +2583,8 @@
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A129" s="8">
-        <v>44059</v>
+      <c r="A129" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>13</v>
@@ -2587,8 +2597,8 @@
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A130" s="8">
-        <v>44059</v>
+      <c r="A130" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>13</v>
@@ -2601,8 +2611,8 @@
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A131" s="8">
-        <v>44059</v>
+      <c r="A131" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>13</v>
@@ -2615,8 +2625,8 @@
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A132" s="8">
-        <v>44059</v>
+      <c r="A132" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>13</v>
@@ -2629,8 +2639,8 @@
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A133" s="8">
-        <v>44059</v>
+      <c r="A133" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>13</v>
@@ -2643,8 +2653,8 @@
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A134" s="8">
-        <v>44059</v>
+      <c r="A134" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>13</v>
@@ -2657,8 +2667,8 @@
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A135" s="8">
-        <v>44059</v>
+      <c r="A135" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>13</v>
@@ -2671,8 +2681,8 @@
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A136" s="8">
-        <v>44028</v>
+      <c r="A136" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>0</v>
@@ -2685,8 +2695,8 @@
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A137" s="8">
-        <v>44028</v>
+      <c r="A137" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>6</v>
@@ -2699,8 +2709,8 @@
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A138" s="8">
-        <v>44028</v>
+      <c r="A138" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>6</v>
@@ -2713,8 +2723,8 @@
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A139" s="8">
-        <v>44028</v>
+      <c r="A139" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>6</v>
@@ -2727,8 +2737,8 @@
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A140" s="8">
-        <v>44028</v>
+      <c r="A140" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>1</v>
@@ -2741,8 +2751,8 @@
       </c>
     </row>
     <row r="141" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="8">
-        <v>44028</v>
+      <c r="A141" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>1</v>
@@ -2755,8 +2765,8 @@
       </c>
     </row>
     <row r="142" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="8">
-        <v>44028</v>
+      <c r="A142" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>1</v>
@@ -2774,8 +2784,8 @@
       <c r="L142" s="7"/>
     </row>
     <row r="143" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="8">
-        <v>44028</v>
+      <c r="A143" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>1</v>
@@ -2793,8 +2803,8 @@
       <c r="L143" s="7"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A144" s="8">
-        <v>44028</v>
+      <c r="A144" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>1</v>
@@ -2807,8 +2817,8 @@
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A145" s="8">
-        <v>44028</v>
+      <c r="A145" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>1</v>
@@ -2821,8 +2831,8 @@
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A146" s="8">
-        <v>44028</v>
+      <c r="A146" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>1</v>
@@ -2835,8 +2845,8 @@
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A147" s="8">
-        <v>44028</v>
+      <c r="A147" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>1</v>
@@ -2849,8 +2859,8 @@
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A148" s="8">
-        <v>44028</v>
+      <c r="A148" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>1</v>
@@ -2863,8 +2873,8 @@
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A149" s="8">
-        <v>44028</v>
+      <c r="A149" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>1</v>
@@ -2877,8 +2887,8 @@
       </c>
     </row>
     <row r="150" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="8">
-        <v>44028</v>
+      <c r="A150" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>7</v>
@@ -2887,12 +2897,12 @@
         <v>25</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="8">
-        <v>44028</v>
+      <c r="A151" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>7</v>
@@ -2910,8 +2920,8 @@
       <c r="K151" s="7"/>
     </row>
     <row r="152" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="8">
-        <v>44028</v>
+      <c r="A152" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>7</v>
@@ -2929,8 +2939,8 @@
       <c r="K152" s="7"/>
     </row>
     <row r="153" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="8">
-        <v>44028</v>
+      <c r="A153" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>7</v>
@@ -2948,8 +2958,8 @@
       <c r="K153" s="7"/>
     </row>
     <row r="154" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="8">
-        <v>44028</v>
+      <c r="A154" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>7</v>
@@ -2958,7 +2968,7 @@
         <v>25</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G154" s="7"/>
       <c r="H154" s="7"/>
@@ -2967,8 +2977,8 @@
       <c r="K154" s="7"/>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A155" s="8">
-        <v>44028</v>
+      <c r="A155" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>7</v>
@@ -2981,8 +2991,8 @@
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A156" s="8">
-        <v>44028</v>
+      <c r="A156" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>7</v>
@@ -2995,8 +3005,8 @@
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A157" s="8">
-        <v>44028</v>
+      <c r="A157" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>7</v>
@@ -3009,8 +3019,8 @@
       </c>
     </row>
     <row r="158" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A158" s="8">
-        <v>44028</v>
+      <c r="A158" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>7</v>
@@ -3019,12 +3029,12 @@
         <v>25</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A159" s="8">
-        <v>44028</v>
+      <c r="A159" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>7</v>
@@ -3037,8 +3047,8 @@
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A160" s="8">
-        <v>44028</v>
+      <c r="A160" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>7</v>
@@ -3051,8 +3061,8 @@
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A161" s="8">
-        <v>44028</v>
+      <c r="A161" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>7</v>
@@ -3065,8 +3075,8 @@
       </c>
     </row>
     <row r="162" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="8">
-        <v>44028</v>
+      <c r="A162" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>7</v>
@@ -3079,8 +3089,8 @@
       </c>
     </row>
     <row r="163" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="8">
-        <v>44028</v>
+      <c r="A163" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>7</v>
@@ -3098,8 +3108,8 @@
       <c r="L163" s="7"/>
     </row>
     <row r="164" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="8">
-        <v>44028</v>
+      <c r="A164" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>7</v>
@@ -3117,8 +3127,8 @@
       <c r="L164" s="7"/>
     </row>
     <row r="165" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="8">
-        <v>44028</v>
+      <c r="A165" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>7</v>
@@ -3136,8 +3146,8 @@
       <c r="L165" s="7"/>
     </row>
     <row r="166" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="8">
-        <v>44028</v>
+      <c r="A166" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>7</v>
@@ -3155,8 +3165,8 @@
       <c r="L166" s="7"/>
     </row>
     <row r="167" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="8">
-        <v>44028</v>
+      <c r="A167" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>7</v>
@@ -3174,8 +3184,8 @@
       <c r="L167" s="7"/>
     </row>
     <row r="168" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="8">
-        <v>44028</v>
+      <c r="A168" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>7</v>
@@ -3193,8 +3203,8 @@
       <c r="L168" s="7"/>
     </row>
     <row r="169" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="8">
-        <v>44028</v>
+      <c r="A169" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>7</v>
@@ -3212,8 +3222,8 @@
       <c r="L169" s="7"/>
     </row>
     <row r="170" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="8">
-        <v>44028</v>
+      <c r="A170" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>13</v>
@@ -3222,7 +3232,7 @@
         <v>26</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
@@ -3231,8 +3241,8 @@
       <c r="L170" s="7"/>
     </row>
     <row r="171" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="8">
-        <v>44028</v>
+      <c r="A171" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>13</v>
@@ -3241,7 +3251,7 @@
         <v>26</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
@@ -3250,8 +3260,8 @@
       <c r="L171" s="7"/>
     </row>
     <row r="172" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="8">
-        <v>44028</v>
+      <c r="A172" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>13</v>
@@ -3269,8 +3279,8 @@
       <c r="L172" s="7"/>
     </row>
     <row r="173" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="8">
-        <v>44028</v>
+      <c r="A173" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>13</v>
@@ -3288,8 +3298,8 @@
       <c r="L173" s="7"/>
     </row>
     <row r="174" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="8">
-        <v>44028</v>
+      <c r="A174" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>13</v>
@@ -3307,8 +3317,8 @@
       <c r="L174" s="7"/>
     </row>
     <row r="175" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="8">
-        <v>44028</v>
+      <c r="A175" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>13</v>
@@ -3326,8 +3336,8 @@
       <c r="L175" s="7"/>
     </row>
     <row r="176" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="8">
-        <v>44028</v>
+      <c r="A176" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>13</v>
@@ -3345,8 +3355,8 @@
       <c r="L176" s="7"/>
     </row>
     <row r="177" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="8">
-        <v>44028</v>
+      <c r="A177" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>13</v>
@@ -3364,8 +3374,8 @@
       <c r="L177" s="7"/>
     </row>
     <row r="178" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="8">
-        <v>44028</v>
+      <c r="A178" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>13</v>
@@ -3383,8 +3393,8 @@
       <c r="L178" s="7"/>
     </row>
     <row r="179" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="8">
-        <v>44028</v>
+      <c r="A179" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>13</v>
@@ -3402,8 +3412,8 @@
       <c r="L179" s="7"/>
     </row>
     <row r="180" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="8">
-        <v>44028</v>
+      <c r="A180" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>13</v>
@@ -3421,8 +3431,8 @@
       <c r="L180" s="7"/>
     </row>
     <row r="181" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="8">
-        <v>44028</v>
+      <c r="A181" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>13</v>
@@ -3440,8 +3450,8 @@
       <c r="L181" s="7"/>
     </row>
     <row r="182" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="8">
-        <v>44028</v>
+      <c r="A182" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>13</v>
@@ -3459,8 +3469,8 @@
       <c r="L182" s="7"/>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A183" s="8">
-        <v>44028</v>
+      <c r="A183" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>13</v>
@@ -3473,8 +3483,8 @@
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A184" s="8">
-        <v>44028</v>
+      <c r="A184" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>13</v>
@@ -3487,8 +3497,8 @@
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A185" s="8">
-        <v>44028</v>
+      <c r="A185" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>13</v>
@@ -3501,8 +3511,8 @@
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A186" s="8">
-        <v>44028</v>
+      <c r="A186" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>13</v>
@@ -3515,8 +3525,8 @@
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A187" s="8">
-        <v>44028</v>
+      <c r="A187" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>13</v>
@@ -3529,8 +3539,8 @@
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A188" s="8">
-        <v>44028</v>
+      <c r="A188" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>13</v>
@@ -3543,8 +3553,8 @@
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A189" s="8">
-        <v>44028</v>
+      <c r="A189" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>13</v>
@@ -3557,8 +3567,8 @@
       </c>
     </row>
     <row r="190" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A190" s="8">
-        <v>44028</v>
+      <c r="A190" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>13</v>
@@ -3567,12 +3577,12 @@
         <v>26</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="191" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A191" s="8">
-        <v>44028</v>
+      <c r="A191" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>13</v>
@@ -3581,12 +3591,12 @@
         <v>26</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A192" s="8">
-        <v>44028</v>
+      <c r="A192" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>13</v>
@@ -3599,8 +3609,8 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A193" s="8">
-        <v>44028</v>
+      <c r="A193" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>13</v>
@@ -3613,8 +3623,8 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A194" s="8">
-        <v>44028</v>
+      <c r="A194" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>13</v>
@@ -3627,8 +3637,8 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A195" s="8">
-        <v>44028</v>
+      <c r="A195" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>13</v>
@@ -3641,8 +3651,8 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A196" s="8">
-        <v>44028</v>
+      <c r="A196" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>13</v>
@@ -3655,8 +3665,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A197" s="8">
-        <v>44028</v>
+      <c r="A197" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>13</v>
@@ -3669,8 +3679,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A198" s="8">
-        <v>44028</v>
+      <c r="A198" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>13</v>
@@ -3683,8 +3693,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A199" s="8">
-        <v>44028</v>
+      <c r="A199" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>13</v>
@@ -3697,8 +3707,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A200" s="8">
-        <v>44028</v>
+      <c r="A200" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>13</v>
@@ -3711,8 +3721,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A201" s="8">
-        <v>44028</v>
+      <c r="A201" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>13</v>
@@ -3725,8 +3735,8 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A202" s="8">
-        <v>44028</v>
+      <c r="A202" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>13</v>
@@ -3739,8 +3749,8 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A203" s="8">
-        <v>44028</v>
+      <c r="A203" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>13</v>
@@ -3753,8 +3763,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" s="8">
-        <v>44028</v>
+      <c r="A204" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>13</v>
@@ -3767,8 +3777,8 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A205" s="8">
-        <v>44028</v>
+      <c r="A205" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>13</v>
@@ -3781,8 +3791,8 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A206" s="8">
-        <v>44028</v>
+      <c r="A206" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>13</v>
@@ -3795,8 +3805,8 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A207" s="8">
-        <v>44028</v>
+      <c r="A207" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>13</v>
@@ -3809,8 +3819,8 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A208" s="8">
-        <v>44028</v>
+      <c r="A208" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>13</v>
@@ -3823,8 +3833,8 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A209" s="8">
-        <v>44028</v>
+      <c r="A209" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>13</v>
@@ -3837,8 +3847,8 @@
       </c>
     </row>
     <row r="210" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A210" s="8">
-        <v>44028</v>
+      <c r="A210" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>13</v>
@@ -3847,12 +3857,12 @@
         <v>26</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A211" s="8">
-        <v>44028</v>
+      <c r="A211" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>13</v>
@@ -3861,12 +3871,12 @@
         <v>26</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A212" s="8">
-        <v>44028</v>
+      <c r="A212" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>13</v>
@@ -3879,8 +3889,8 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A213" s="8">
-        <v>44028</v>
+      <c r="A213" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>13</v>
@@ -3893,8 +3903,8 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A214" s="8">
-        <v>44028</v>
+      <c r="A214" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>13</v>
@@ -3907,8 +3917,8 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" s="8">
-        <v>44028</v>
+      <c r="A215" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>13</v>
@@ -3921,8 +3931,8 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" s="8">
-        <v>44028</v>
+      <c r="A216" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>13</v>
@@ -3935,8 +3945,8 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" s="8">
-        <v>44028</v>
+      <c r="A217" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>13</v>
@@ -3949,8 +3959,8 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218" s="8">
-        <v>44028</v>
+      <c r="A218" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>13</v>
@@ -3963,8 +3973,8 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A219" s="8">
-        <v>44028</v>
+      <c r="A219" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>13</v>
@@ -3977,8 +3987,8 @@
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" s="8">
-        <v>44028</v>
+      <c r="A220" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>13</v>
@@ -3991,8 +4001,8 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A221" s="8">
-        <v>44028</v>
+      <c r="A221" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>13</v>
@@ -4005,8 +4015,8 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A222" s="8">
-        <v>44028</v>
+      <c r="A222" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>13</v>
@@ -4019,8 +4029,8 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A223" s="8">
-        <v>44028</v>
+      <c r="A223" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>13</v>
@@ -4033,8 +4043,8 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" s="8">
-        <v>44028</v>
+      <c r="A224" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>13</v>
@@ -4047,8 +4057,8 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" s="8">
-        <v>44028</v>
+      <c r="A225" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>13</v>
@@ -4061,8 +4071,8 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A226" s="8">
-        <v>44028</v>
+      <c r="A226" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>13</v>
@@ -4075,8 +4085,8 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A227" s="8">
-        <v>44028</v>
+      <c r="A227" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>13</v>
@@ -4089,8 +4099,8 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A228" s="8">
-        <v>44028</v>
+      <c r="A228" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>13</v>
@@ -4103,8 +4113,8 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A229" s="8">
-        <v>44028</v>
+      <c r="A229" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>13</v>
@@ -4117,8 +4127,8 @@
       </c>
     </row>
     <row r="230" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A230" s="8">
-        <v>44028</v>
+      <c r="A230" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>13</v>
@@ -4127,26 +4137,26 @@
         <v>26</v>
       </c>
       <c r="D230" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A231" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D231" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A231" s="8">
-        <v>44028</v>
-      </c>
-      <c r="B231" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D231" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232" s="8">
-        <v>44028</v>
+      <c r="A232" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>13</v>
@@ -4159,8 +4169,8 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A233" s="8">
-        <v>44028</v>
+      <c r="A233" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>13</v>
@@ -4173,8 +4183,8 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" s="8">
-        <v>44028</v>
+      <c r="A234" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>13</v>
@@ -4187,8 +4197,8 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" s="8">
-        <v>44028</v>
+      <c r="A235" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>13</v>
@@ -4201,8 +4211,8 @@
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="8">
-        <v>44028</v>
+      <c r="A236" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>13</v>
@@ -4215,8 +4225,8 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" s="8">
-        <v>44028</v>
+      <c r="A237" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>13</v>
@@ -4229,8 +4239,8 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A238" s="8">
-        <v>44028</v>
+      <c r="A238" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>13</v>
@@ -4243,8 +4253,8 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="8">
-        <v>44028</v>
+      <c r="A239" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>13</v>
@@ -4257,8 +4267,8 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="8">
-        <v>44028</v>
+      <c r="A240" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>13</v>
@@ -4271,8 +4281,8 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A241" s="8">
-        <v>44028</v>
+      <c r="A241" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>13</v>
@@ -4285,8 +4295,8 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A242" s="8">
-        <v>44028</v>
+      <c r="A242" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>13</v>
@@ -4299,8 +4309,8 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A243" s="8">
-        <v>44028</v>
+      <c r="A243" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>13</v>
@@ -4313,8 +4323,8 @@
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A244" s="8">
-        <v>44028</v>
+      <c r="A244" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>13</v>
@@ -4327,8 +4337,8 @@
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A245" s="8">
-        <v>44028</v>
+      <c r="A245" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>13</v>
@@ -4341,8 +4351,8 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246" s="8">
-        <v>44028</v>
+      <c r="A246" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>13</v>
@@ -4355,8 +4365,8 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" s="8">
-        <v>44028</v>
+      <c r="A247" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>13</v>
@@ -4369,8 +4379,8 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248" s="8">
-        <v>44028</v>
+      <c r="A248" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>13</v>
@@ -4383,8 +4393,8 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A249" s="8">
-        <v>44028</v>
+      <c r="A249" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>13</v>
@@ -4397,8 +4407,8 @@
       </c>
     </row>
     <row r="250" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A250" s="8">
-        <v>44028</v>
+      <c r="A250" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>13</v>
@@ -4407,26 +4417,26 @@
         <v>26</v>
       </c>
       <c r="D250" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A251" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D251" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A251" s="8">
-        <v>44028</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D251" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" s="8">
-        <v>44028</v>
+      <c r="A252" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>13</v>
@@ -4439,8 +4449,8 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" s="8">
-        <v>44028</v>
+      <c r="A253" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>13</v>
@@ -4453,8 +4463,8 @@
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A254" s="8">
-        <v>44028</v>
+      <c r="A254" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>13</v>
@@ -4467,8 +4477,8 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A255" s="8">
-        <v>44028</v>
+      <c r="A255" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B255" s="3" t="s">
         <v>13</v>
@@ -4481,8 +4491,8 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" s="8">
-        <v>44028</v>
+      <c r="A256" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>13</v>
@@ -4495,8 +4505,8 @@
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A257" s="8">
-        <v>44028</v>
+      <c r="A257" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>13</v>
@@ -4509,8 +4519,8 @@
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A258" s="8">
-        <v>44028</v>
+      <c r="A258" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B258" s="3" t="s">
         <v>13</v>
@@ -4523,8 +4533,8 @@
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A259" s="8">
-        <v>44028</v>
+      <c r="A259" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B259" s="3" t="s">
         <v>13</v>
@@ -4537,8 +4547,8 @@
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A260" s="8">
-        <v>44028</v>
+      <c r="A260" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>13</v>
@@ -4551,8 +4561,8 @@
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A261" s="8">
-        <v>44028</v>
+      <c r="A261" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>13</v>
@@ -4565,8 +4575,8 @@
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A262" s="8">
-        <v>44028</v>
+      <c r="A262" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>13</v>
@@ -4579,8 +4589,8 @@
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A263" s="8">
-        <v>44028</v>
+      <c r="A263" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>13</v>
@@ -4593,8 +4603,8 @@
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A264" s="8">
-        <v>44028</v>
+      <c r="A264" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>13</v>
@@ -4607,8 +4617,8 @@
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A265" s="8">
-        <v>44028</v>
+      <c r="A265" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>13</v>
@@ -4621,8 +4631,8 @@
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A266" s="8">
-        <v>44028</v>
+      <c r="A266" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B266" s="3" t="s">
         <v>13</v>
@@ -4635,8 +4645,8 @@
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A267" s="8">
-        <v>44028</v>
+      <c r="A267" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B267" s="3" t="s">
         <v>13</v>
@@ -4649,8 +4659,8 @@
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A268" s="8">
-        <v>44028</v>
+      <c r="A268" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B268" s="3" t="s">
         <v>13</v>
@@ -4663,8 +4673,8 @@
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A269" s="8">
-        <v>44028</v>
+      <c r="A269" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B269" s="3" t="s">
         <v>13</v>
@@ -4677,6 +4687,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>